<commit_message>
added PDF generation from xml risk session data
</commit_message>
<xml_diff>
--- a/riscoss-webapp/src/main/webapp/resources/entities_info.xlsx
+++ b/riscoss-webapp/src/main/webapp/resources/entities_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="115" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="IPR Registry" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Entities" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="OSS Licenses" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
-  <si>
-    <t>IPR Registry</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
+  <si>
+    <t>Entities</t>
   </si>
   <si>
     <t>#</t>
@@ -58,87 +58,108 @@
     <t>Last update</t>
   </si>
   <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>ASL3</t>
-  </si>
-  <si>
-    <t>b1</t>
+    <t>riscoss-corporate</t>
   </si>
   <si>
     <t>ASL2</t>
   </si>
   <si>
-    <t>c1</t>
+    <t>GWT</t>
+  </si>
+  <si>
+    <t>Junit</t>
+  </si>
+  <si>
+    <t>CPL-EPL</t>
+  </si>
+  <si>
+    <t>GFLOT</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>FOP</t>
+  </si>
+  <si>
+    <t>POI</t>
+  </si>
+  <si>
+    <t>RestyGWT</t>
+  </si>
+  <si>
+    <t>JAX-RS</t>
+  </si>
+  <si>
+    <t>CDDL</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>GWTUpload</t>
+  </si>
+  <si>
+    <t>Apache Commons</t>
+  </si>
+  <si>
+    <t>GSON</t>
+  </si>
+  <si>
+    <t>OrientDB</t>
+  </si>
+  <si>
+    <t>Apache HTTPComponents</t>
+  </si>
+  <si>
+    <t>License ID</t>
+  </si>
+  <si>
+    <t>License Description</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>The MIT License</t>
+  </si>
+  <si>
+    <t>BSD4</t>
+  </si>
+  <si>
+    <t>The BSD 2-Clause License</t>
+  </si>
+  <si>
+    <t>BSD3</t>
+  </si>
+  <si>
+    <t>The BSD 3-Clause License</t>
+  </si>
+  <si>
+    <t>ASL1</t>
+  </si>
+  <si>
+    <t>Apache License, Version 1.0</t>
+  </si>
+  <si>
+    <t>http://www.apache.org/licenses/</t>
+  </si>
+  <si>
+    <t>Apache License, Version 2.0</t>
   </si>
   <si>
     <t>Artistic2</t>
   </si>
   <si>
-    <t>d1</t>
+    <t>Artistic License 2.0</t>
+  </si>
+  <si>
+    <t>https://tldrlegal.com/license/artistic-license-2.0-(artistic)</t>
   </si>
   <si>
     <t>LGPL2.1</t>
   </si>
   <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>d2</t>
-  </si>
-  <si>
-    <t>License ID</t>
-  </si>
-  <si>
-    <t>License Description</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>MIT</t>
-  </si>
-  <si>
-    <t>The MIT License</t>
-  </si>
-  <si>
-    <t>BSD4</t>
-  </si>
-  <si>
-    <t>The BSD 2-Clause License</t>
-  </si>
-  <si>
-    <t>BSD3</t>
-  </si>
-  <si>
-    <t>The BSD 3-Clause License</t>
-  </si>
-  <si>
-    <t>ASL1</t>
-  </si>
-  <si>
-    <t>Apache License, Version 1.0</t>
-  </si>
-  <si>
-    <t>http://www.apache.org/licenses/</t>
-  </si>
-  <si>
-    <t>Apache License, Version 2.0</t>
-  </si>
-  <si>
-    <t>Artistic License 2.0</t>
-  </si>
-  <si>
-    <t>https://tldrlegal.com/license/artistic-license-2.0-(artistic)</t>
-  </si>
-  <si>
     <t>The GNU Lesser General Public License, version 2.1</t>
   </si>
   <si>
@@ -160,13 +181,7 @@
     <t>Mozilla Public License</t>
   </si>
   <si>
-    <t>CDDL</t>
-  </si>
-  <si>
     <t>Common Development and Distribution License</t>
-  </si>
-  <si>
-    <t>CPL-EPL</t>
   </si>
   <si>
     <t>Eclipse Public License</t>
@@ -355,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,6 +409,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -484,50 +503,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>230040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>20520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>542520</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Bild 5" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="572760" y="20520"/>
-          <a:ext cx="2742120" cy="471600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -536,17 +511,17 @@
   <dimension ref="1:68"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.2908163265306"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.9795918367347"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7091836734694"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.8622448979592"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.7040816326531"/>
@@ -3682,9 +3657,7 @@
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
         <v>14</v>
       </c>
@@ -3694,11 +3667,9 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <v>1</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="9"/>
@@ -3714,15 +3685,13 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v>1</v>
-      </c>
+      <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="9"/>
@@ -3738,15 +3707,13 @@
       <c r="D9" s="0"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="8" t="n">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I9" s="0"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="9"/>
@@ -3756,23 +3723,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="I10" s="11"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
@@ -3782,17 +3745,17 @@
         <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -3804,17 +3767,17 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="0"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="10" t="s">
-        <v>20</v>
+      <c r="H12" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -3822,98 +3785,154 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="H15" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="8"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="8" t="n">
+        <v>12</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -4616,7 +4635,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4628,7 +4646,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="A20:B20 A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4640,167 +4658,167 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>27</v>
+      <c r="A1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>36</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>